<commit_message>
Added checks to create new cell/row if a cell/row is requested that does not already exist in the spreadsheet
</commit_message>
<xml_diff>
--- a/src/main/resources/invoiceTemplate.xlsx
+++ b/src/main/resources/invoiceTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="timesheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Name:</t>
   </si>
@@ -39,7 +39,7 @@
     <t>Project Code</t>
   </si>
   <si>
-    <t>Project Name, Role, and Story Card </t>
+    <t>Project Name, Role, and Story Card</t>
   </si>
   <si>
     <t>Sat</t>
@@ -102,9 +102,6 @@
     <t>Omnicrola LLC</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>[PERSONAL DATA]</t>
   </si>
   <si>
@@ -169,16 +166,13 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Make all checks payable to Omnicrola LLC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YYYY;@"/>
@@ -188,7 +182,6 @@
     <numFmt numFmtId="170" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="171" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="172" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="173" formatCode="\$#,##0.00"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -782,7 +775,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="113">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -923,10 +916,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1235,11 +1224,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1320,15 +1305,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>322560</xdr:colOff>
+      <xdr:colOff>349560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>569880</xdr:colOff>
+      <xdr:colOff>596520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1343,8 +1328,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8113680" y="143280"/>
-          <a:ext cx="1668600" cy="555840"/>
+          <a:off x="8140680" y="134280"/>
+          <a:ext cx="1668240" cy="555480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1366,7 +1351,7 @@
   </sheetPr>
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1549,29 +1534,29 @@
       <c r="B6" s="26"/>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
-      <c r="E6" s="32" t="e">
+      <c r="E6" s="32" t="n">
         <f aca="false">IF(($C$3=""),"",(F6-1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F6" s="32" t="e">
+        <v>-6</v>
+      </c>
+      <c r="F6" s="32" t="n">
         <f aca="false">IF(($C$3=""),"",(G6-1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G6" s="32" t="e">
+        <v>-5</v>
+      </c>
+      <c r="G6" s="32" t="n">
         <f aca="false">IF(($C$3=""),"",(H6-1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H6" s="32" t="e">
+        <v>-4</v>
+      </c>
+      <c r="H6" s="32" t="n">
         <f aca="false">IF(($C$3=""),"",(I6-1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I6" s="32" t="e">
+        <v>-3</v>
+      </c>
+      <c r="I6" s="32" t="n">
         <f aca="false">IF(($C$3=""),"",(J6-1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J6" s="32" t="e">
+        <v>-2</v>
+      </c>
+      <c r="J6" s="32" t="n">
         <f aca="false">IF(($C$3=""),"",(K6-1))</f>
-        <v>#VALUE!</v>
+        <v>-1</v>
       </c>
       <c r="K6" s="32" t="n">
         <f aca="false">IF(($C$3=""),"",C3)</f>
@@ -1595,26 +1580,26 @@
       <c r="AA6" s="13"/>
       <c r="AB6" s="13"/>
     </row>
-    <row r="7" s="42" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" s="41" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="33"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="39" t="n">
+      <c r="D7" s="8"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="38" t="n">
         <f aca="false">SUM(E7:K7)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="40"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
       <c r="S7" s="13"/>
@@ -1629,32 +1614,32 @@
       <c r="AB7" s="13"/>
     </row>
     <row r="8" s="14" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="47" t="s">
+      <c r="A8" s="42"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="48" t="n">
+      <c r="L8" s="47" t="n">
         <f aca="false">SUM(L7:L7)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="49"/>
+      <c r="M8" s="48"/>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43"/>
-      <c r="B9" s="50" t="s">
+      <c r="A9" s="42"/>
+      <c r="B9" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="12"/>
@@ -1667,168 +1652,168 @@
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-      <c r="M9" s="49"/>
+      <c r="M9" s="48"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="39" t="n">
+      <c r="D10" s="8"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="38" t="n">
         <f aca="false">SUM(E10:K10)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="49"/>
+      <c r="M10" s="48"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="13"/>
     </row>
     <row r="11" s="14" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="47" t="s">
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="48" t="e">
+      <c r="L11" s="47" t="n">
         <f aca="false">SUM(L8:L8)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M11" s="49"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="48"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="13"/>
     </row>
-    <row r="12" s="42" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51"/>
-      <c r="B12" s="50" t="s">
+    <row r="12" s="41" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="50"/>
+      <c r="B12" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="55"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="54"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="51"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="39" t="n">
+      <c r="D13" s="8"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="38" t="n">
         <f aca="false">SUM(E13:K13)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="54" t="n">
-        <f aca="false">SUM(L19:L13)</f>
+      <c r="M13" s="53" t="n">
+        <f aca="false">SUM(L13:L19)</f>
         <v>0</v>
       </c>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="55"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="54"/>
     </row>
     <row r="14" s="14" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="43"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="47" t="s">
+      <c r="A14" s="42"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="48" t="n">
+      <c r="L14" s="47" t="n">
         <f aca="false">SUM(L13:L13)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="49"/>
+      <c r="M14" s="48"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="43"/>
-      <c r="B15" s="56"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="57" t="s">
+      <c r="D15" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="58" t="n">
+      <c r="E15" s="57" t="n">
         <f aca="false">SUM(E7:E13)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="58" t="n">
+      <c r="F15" s="57" t="n">
         <f aca="false">SUM(F7:F13)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="58" t="n">
+      <c r="G15" s="57" t="n">
         <f aca="false">SUM(G7:G13)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="58" t="n">
+      <c r="H15" s="57" t="n">
         <f aca="false">SUM(H7:H13)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="58" t="n">
+      <c r="I15" s="57" t="n">
         <f aca="false">SUM(I7:I13)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="58" t="n">
+      <c r="J15" s="57" t="n">
         <f aca="false">SUM(J7:J13)</f>
         <v>0</v>
       </c>
-      <c r="K15" s="58" t="n">
+      <c r="K15" s="57" t="n">
         <f aca="false">SUM(K7:K13)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="59" t="n">
+      <c r="L15" s="58" t="n">
         <f aca="false">SUM(E15:K15)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="60"/>
+      <c r="M15" s="59"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="12"/>
@@ -1836,43 +1821,43 @@
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18"/>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="63"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="65"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="64"/>
       <c r="P16" s="24"/>
-      <c r="Q16" s="65"/>
+      <c r="Q16" s="64"/>
     </row>
     <row r="17" s="14" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6"/>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="68" t="s">
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="64"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="63"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="12"/>
@@ -1880,18 +1865,18 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="64"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="63"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="12"/>
@@ -1899,17 +1884,17 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
       <c r="M19" s="11"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
@@ -1918,24 +1903,24 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
-      <c r="B20" s="69" t="s">
+      <c r="B20" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="70" t="n">
+      <c r="C20" s="69" t="n">
         <f aca="false">C3</f>
         <v>0</v>
       </c>
-      <c r="D20" s="70"/>
-      <c r="E20" s="71" t="s">
+      <c r="D20" s="69"/>
+      <c r="E20" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="71"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
       <c r="M20" s="11"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
@@ -1943,23 +1928,23 @@
       <c r="Q20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="72"/>
-      <c r="B21" s="73"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="76"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="75"/>
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
       <c r="P21" s="24"/>
-      <c r="Q21" s="65"/>
+      <c r="Q21" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1994,8 +1979,8 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2012,230 +1997,211 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
     </row>
     <row r="3" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="J3" s="82" t="s">
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="J3" s="81"/>
+    </row>
+    <row r="4" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="82" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="83" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="84" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="85" t="n">
+      <c r="F4" s="84" t="n">
         <f aca="false">timesheet!C3</f>
         <v>0</v>
       </c>
-      <c r="J4" s="86"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="86" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="87"/>
+    </row>
+    <row r="6" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="88"/>
-    </row>
-    <row r="6" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="89" t="s">
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="90"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="79"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="79"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="91"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="80"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="80"/>
-    </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="92" t="s">
+      <c r="C8" s="91"/>
+      <c r="E8" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="E8" s="92" t="s">
+      <c r="F8" s="92"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="93"/>
-    </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="94" t="s">
+      <c r="C9" s="93"/>
+      <c r="E9" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="94"/>
-      <c r="E9" s="94" t="s">
+      <c r="F9" s="94"/>
+    </row>
+    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="95"/>
-    </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="94" t="s">
+      <c r="C10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="94"/>
+    </row>
+    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="95"/>
-    </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="94" t="s">
+      <c r="C11" s="95"/>
+      <c r="E11" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="96"/>
-      <c r="E11" s="94" t="s">
+      <c r="F11" s="96"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="97"/>
-    </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="94" t="s">
+      <c r="C12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="96"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="94"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="97"/>
-    </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="94" t="s">
+      <c r="C13" s="93"/>
+      <c r="E13" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="94"/>
-      <c r="E13" s="94" t="s">
+      <c r="F13" s="96"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="93"/>
+      <c r="C14" s="95"/>
+      <c r="E14" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="97"/>
-    </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="94"/>
-      <c r="C14" s="96"/>
-      <c r="E14" s="94" t="s">
+      <c r="F14" s="96"/>
+    </row>
+    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="93"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="96"/>
+    </row>
+    <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="93"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="96"/>
+    </row>
+    <row r="17" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="97"/>
-    </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="94"/>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="97"/>
-    </row>
-    <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="94"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="97"/>
-    </row>
-    <row r="17" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="99" t="s">
+      <c r="B17" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="100" t="s">
+      <c r="C17" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="100" t="s">
+      <c r="D17" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="101" t="s">
+      <c r="E17" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="102" t="s">
+      <c r="F17" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="103" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="103"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="108"/>
+    </row>
+    <row r="19" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="77"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="111" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="104"/>
-      <c r="B18" s="105"/>
-      <c r="C18" s="106"/>
-      <c r="D18" s="107"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="109"/>
-    </row>
-    <row r="19" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="78"/>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="112" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="113" t="n">
+      <c r="F19" s="112" t="n">
         <f aca="false">SUM(F18:F18)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="81"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="114" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="114"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="114"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="114"/>
-    </row>
+    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A21:F21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>